<commit_message>
Updated Marathi Name split logic
</commit_message>
<xml_diff>
--- a/141_Data/Progress of pdfs.xlsx
+++ b/141_Data/Progress of pdfs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sahil_Tejam\ALL_OCR\Marathi_OCR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sahil_Tejam\ALL_OCR\Marathi_OCR\141_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68910873-E3DA-487F-A0B4-97CCA513B609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C407A1-2673-4BF6-BE8B-83355F16EE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2EB75618-E09B-4366-A084-492205DB3AFD}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{2EB75618-E09B-4366-A084-492205DB3AFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t>AC_NO</t>
   </si>
@@ -53,9 +53,6 @@
   <si>
     <t>Completed</t>
   </si>
-  <si>
-    <t>In Progress</t>
-  </si>
 </sst>
 </file>
 
@@ -70,12 +67,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -90,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B4C1DE-8331-4362-9F82-E77A882DDCBC}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +424,7 @@
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,14 +441,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>143</v>
       </c>
       <c r="B2">
         <v>25763</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>2123</v>
       </c>
       <c r="D2">
@@ -454,14 +458,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>139</v>
       </c>
       <c r="B3">
         <v>25128</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1192</v>
       </c>
       <c r="D3">
@@ -471,14 +475,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>142</v>
       </c>
       <c r="B4">
         <v>25445</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1557</v>
       </c>
       <c r="D4">
@@ -488,14 +492,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>144</v>
       </c>
       <c r="B5">
         <v>42179</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>3035</v>
       </c>
       <c r="D5">
@@ -505,14 +509,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>138</v>
       </c>
       <c r="B6">
         <v>28994</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>3714</v>
       </c>
       <c r="D6">
@@ -522,174 +526,167 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B7">
-        <v>25128</v>
-      </c>
-      <c r="C7">
-        <v>1192</v>
+        <v>9328</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1101</v>
       </c>
       <c r="D7">
-        <v>6526</v>
+        <v>4359</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B8">
-        <v>9328</v>
+        <v>16435</v>
       </c>
       <c r="C8">
-        <v>1101</v>
+        <v>1581</v>
       </c>
       <c r="D8">
-        <v>4359</v>
+        <v>3874</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B9">
-        <v>1925</v>
-      </c>
-      <c r="C9">
-        <v>288</v>
+        <v>36579</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4512</v>
       </c>
       <c r="D9">
-        <v>415</v>
+        <v>6597</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B10">
-        <v>36579</v>
-      </c>
-      <c r="C10">
-        <v>4512</v>
+        <v>9056</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2982</v>
       </c>
       <c r="D10">
-        <v>6597</v>
+        <v>4750</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f>1293+1006</f>
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B11">
-        <v>9056</v>
-      </c>
-      <c r="C11">
-        <v>2982</v>
+        <v>19751</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2258</v>
       </c>
       <c r="D11">
-        <v>4750</v>
+        <v>5537</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B12">
-        <v>19751</v>
-      </c>
-      <c r="C12">
-        <v>2258</v>
+        <v>21114</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8203</v>
       </c>
       <c r="D12">
-        <v>5537</v>
+        <v>9700</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B13">
-        <v>21114</v>
-      </c>
-      <c r="C13">
-        <v>8203</v>
+        <v>16891</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4715</v>
       </c>
       <c r="D13">
-        <v>9700</v>
+        <v>6995</v>
       </c>
       <c r="E13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B14">
         <v>21855</v>
       </c>
-      <c r="C14">
-        <v>4715</v>
+      <c r="C14" s="1">
+        <v>2516</v>
       </c>
       <c r="D14">
-        <v>6995</v>
+        <v>5504</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>151</v>
+        <v>188</v>
       </c>
       <c r="B15">
-        <v>21855</v>
-      </c>
-      <c r="C15">
-        <v>2516</v>
+        <v>34365</v>
+      </c>
+      <c r="C15" s="1">
+        <v>4121</v>
       </c>
       <c r="D15">
-        <v>5504</v>
+        <v>9733</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>188</v>
-      </c>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>34365</v>
-      </c>
-      <c r="C16">
-        <v>4121</v>
-      </c>
-      <c r="D16">
-        <v>9733</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
+        <f>SUM(B2:B15)</f>
+        <v>332883</v>
       </c>
     </row>
   </sheetData>

</xml_diff>